<commit_message>
added the weekly report+updated minute meetings
</commit_message>
<xml_diff>
--- a/documentation/PlanningPhase/CS673F13P4_weeklyreport.xlsx
+++ b/documentation/PlanningPhase/CS673F13P4_weeklyreport.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="56">
   <si>
     <t>week #</t>
   </si>
@@ -85,6 +85,11 @@
 6-presentation</t>
   </si>
   <si>
+    <t>2-Design, worked on the UI Framework design.
+3 - Implementation, created a reusable framework using Html5, JQuery, RequireJs, Bootstrap, Kendo client libraries
+5 - Communication/management, communicating  my changes to team. Knowledge transfer of how to use the framework and implementation details.</t>
+  </si>
+  <si>
     <t>Vipul</t>
   </si>
   <si>
@@ -101,6 +106,12 @@
     <t>UI mock ups, polish user stories, create database</t>
   </si>
   <si>
+    <t>0- learning SQL
+1 - database design analysis 
+2 - communication/management 3- database creation 
+</t>
+  </si>
+  <si>
     <t>Vipul Aggarwal</t>
   </si>
   <si>
@@ -127,7 +138,23 @@
 6-presentation</t>
   </si>
   <si>
-    <t>begin developing coponents for task page, bug page and any other reporting pages</t>
+    <t>begin developing components for task page, bug page and any other reporting pages</t>
+  </si>
+  <si>
+    <t>0- learning Kendo UI using Kendo tutorials 
+http://docs.kendoui.com/getting-started/web/appearance-styling
+learning git basics from the following:
+http://git-scm.com/book/en/Git-Branching
+https://github.com/heckendorfc/plm/blob/development/documentation/internal/scmp.pdf
+http://www.youtube.com/watch?v=RDGzF2M-zlo
+http://www.youtube.com/watch?v=mYjZtU1-u9Y
+2 -  worked on the UI Framework design(register,task,bug page)
+3 - created a reusable framework using Html5, JQuery, Kendo client libraries
+5 - Communication/management, communicating  my changes to team.
+</t>
+  </si>
+  <si>
+    <t>implementation of registration, task and bug page</t>
   </si>
   <si>
     <t>Rachit</t>
@@ -139,6 +166,27 @@
 rough draft for the project design </t>
   </si>
   <si>
+    <t>0 – learning about different UI frameworks and basic html.
+1 - requirement analysis 
+2 – design of UML diagrams
+5 - communication/management
+</t>
+  </si>
+  <si>
+    <t>UI mockups and User Stories</t>
+  </si>
+  <si>
+    <t>2-Design, worked on the UI Framework design.
+3 - Implementation, created a reusable framework using Html5, JQuery, RequireJs, Bootstrap, Kendo client libraries
+5 - Communication/management, communicating  my changes to team.</t>
+  </si>
+  <si>
+    <t>Review of previous week
+Update weekly report
+Implementation of Login page
+</t>
+  </si>
+  <si>
     <t>Alan</t>
   </si>
   <si>
@@ -165,6 +213,15 @@
   </si>
   <si>
     <t>Begin developing services</t>
+  </si>
+  <si>
+    <t>0 - Learning required technologies for development (JPA, JAX-RS)
+2 - Developing database schema
+3 - Developing authentication and role management services. Implementing JPA code.
+4 - Writing test cases for services</t>
+  </si>
+  <si>
+    <t>Developing services required for requirements</t>
   </si>
   <si>
     <t>Tandhy</t>
@@ -188,6 +245,15 @@
   <si>
     <t>0 - learning
 6 - work on testing tools</t>
+  </si>
+  <si>
+    <t>0 - learning on selenium, how to install, perform initial test
+2 - draft UI Storyboard
+</t>
+  </si>
+  <si>
+    <t>0 - learning on UnitTesting and database testing
+2 - finish UI Storyboard and work on UI</t>
   </si>
 </sst>
 </file>
@@ -375,6 +441,41 @@
         <v>8</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c t="s" r="B4">
+        <v>15</v>
+      </c>
+      <c r="C4">
+        <v>14</v>
+      </c>
+      <c r="D4">
+        <v>14</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c t="s" r="F4">
+        <v>18</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>2</v>
+      </c>
+      <c r="J4">
+        <v>11</v>
+      </c>
+      <c r="L4">
+        <v>1</v>
+      </c>
+      <c r="N4">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
 </worksheet>
 </file>
@@ -438,7 +539,7 @@
         <v>1</v>
       </c>
       <c t="s" r="B2">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C2">
         <v>7</v>
@@ -450,7 +551,7 @@
         <v>1</v>
       </c>
       <c t="s" r="F2">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G2">
         <v>0</v>
@@ -470,7 +571,7 @@
         <v>2</v>
       </c>
       <c t="s" r="B3">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C3">
         <v>11</v>
@@ -482,7 +583,7 @@
         <v>1</v>
       </c>
       <c t="s" r="F3">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G3">
         <v>4</v>
@@ -506,9 +607,56 @@
         <v>0</v>
       </c>
       <c t="s" r="N3">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="O3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c t="s" r="B4">
+        <v>19</v>
+      </c>
+      <c r="C4">
+        <v>12</v>
+      </c>
+      <c r="D4">
+        <v>11</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c t="s" r="F4">
+        <v>23</v>
+      </c>
+      <c r="G4">
+        <v>2</v>
+      </c>
+      <c r="H4">
+        <v>2</v>
+      </c>
+      <c r="I4">
+        <v>2</v>
+      </c>
+      <c r="J4">
+        <v>5</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>1</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c t="s" r="N4">
+        <v>22</v>
+      </c>
+      <c r="O4">
         <v>10</v>
       </c>
     </row>
@@ -575,7 +723,7 @@
         <v>1</v>
       </c>
       <c t="s" r="B2">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C2">
         <v>7</v>
@@ -587,7 +735,7 @@
         <v>1</v>
       </c>
       <c t="s" r="F2">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G2">
         <v>0</v>
@@ -607,7 +755,7 @@
         <v>2</v>
       </c>
       <c t="s" r="B3">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C3">
         <v>11</v>
@@ -619,7 +767,7 @@
         <v>1</v>
       </c>
       <c t="s" r="F3">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G3">
         <v>5</v>
@@ -643,7 +791,7 @@
         <v>0</v>
       </c>
       <c t="s" r="N3">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="O3">
         <v>10</v>
@@ -659,6 +807,9 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="17.14" defaultRowHeight="12.75"/>
+  <cols>
+    <col min="6" customWidth="1" max="6" width="73.14"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c t="s" r="A1">
@@ -712,7 +863,7 @@
         <v>1</v>
       </c>
       <c t="s" r="B2">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C2">
         <v>7</v>
@@ -724,7 +875,7 @@
         <v>2</v>
       </c>
       <c t="s" r="F2">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="H2">
         <v>2</v>
@@ -733,7 +884,7 @@
         <v>5</v>
       </c>
       <c t="s" r="N2">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="O2">
         <v>7</v>
@@ -744,7 +895,7 @@
         <v>2</v>
       </c>
       <c t="s" r="B3">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C3">
         <v>14</v>
@@ -756,7 +907,7 @@
         <v>1</v>
       </c>
       <c t="s" r="F3">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="G3">
         <v>7</v>
@@ -771,10 +922,48 @@
         <v>2</v>
       </c>
       <c t="s" r="N3">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="O3">
         <v>14</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c t="s" r="B4">
+        <v>26</v>
+      </c>
+      <c r="C4">
+        <v>18</v>
+      </c>
+      <c r="D4">
+        <v>17</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c t="s" r="F4">
+        <v>31</v>
+      </c>
+      <c r="G4">
+        <v>10</v>
+      </c>
+      <c r="I4">
+        <v>3</v>
+      </c>
+      <c r="J4">
+        <v>3</v>
+      </c>
+      <c r="L4">
+        <v>2</v>
+      </c>
+      <c t="s" r="N4">
+        <v>32</v>
+      </c>
+      <c r="O4">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -787,6 +976,10 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="17.14" defaultRowHeight="12.75"/>
+  <cols>
+    <col min="6" customWidth="1" max="6" width="58.0"/>
+    <col min="14" customWidth="1" max="14" width="25.29"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c t="s" r="A1">
@@ -840,7 +1033,7 @@
         <v>1</v>
       </c>
       <c t="s" r="B2">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="C2">
         <v>7</v>
@@ -849,10 +1042,10 @@
         <v>5</v>
       </c>
       <c r="E2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c t="s" r="F2">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="H2">
         <v>2</v>
@@ -861,12 +1054,86 @@
         <v>5</v>
       </c>
       <c t="s" r="N2">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="O2">
-        <v>7</v>
-      </c>
-    </row>
+        <v>10</v>
+      </c>
+    </row>
+    <row customHeight="1" r="3" ht="50.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c t="s" r="B3">
+        <v>33</v>
+      </c>
+      <c r="C3">
+        <v>10</v>
+      </c>
+      <c r="D3">
+        <v>8</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c t="s" r="F3">
+        <v>35</v>
+      </c>
+      <c r="G3">
+        <v>4</v>
+      </c>
+      <c r="H3">
+        <v>2</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="L3">
+        <v>1</v>
+      </c>
+      <c t="s" r="N3">
+        <v>36</v>
+      </c>
+      <c r="O3">
+        <v>15</v>
+      </c>
+    </row>
+    <row customHeight="1" r="4" ht="117.75">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c t="s" r="B4">
+        <v>33</v>
+      </c>
+      <c r="C4">
+        <v>16</v>
+      </c>
+      <c r="D4">
+        <v>15</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c t="s" r="F4">
+        <v>37</v>
+      </c>
+      <c r="I4">
+        <v>2</v>
+      </c>
+      <c r="J4">
+        <v>10</v>
+      </c>
+      <c r="L4">
+        <v>1</v>
+      </c>
+      <c t="s" r="N4">
+        <v>38</v>
+      </c>
+      <c r="O4">
+        <v>20</v>
+      </c>
+    </row>
+    <row customHeight="1" r="5" ht="21.75"/>
   </sheetData>
 </worksheet>
 </file>
@@ -936,7 +1203,7 @@
         <v>1</v>
       </c>
       <c t="s" r="B2">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="C2">
         <v>5</v>
@@ -972,7 +1239,7 @@
         <v>0</v>
       </c>
       <c t="s" r="N2">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="O2">
         <v>5</v>
@@ -983,7 +1250,7 @@
         <v>2</v>
       </c>
       <c t="s" r="B3">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="C3">
         <v>11</v>
@@ -995,7 +1262,7 @@
         <v>1</v>
       </c>
       <c t="s" r="F3">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G3">
         <v>4</v>
@@ -1019,7 +1286,7 @@
         <v>0</v>
       </c>
       <c t="s" r="N3">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="O3">
         <v>10</v>
@@ -1094,7 +1361,7 @@
         <v>1</v>
       </c>
       <c t="s" r="B2">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="C2">
         <v>14</v>
@@ -1106,7 +1373,7 @@
         <v>2</v>
       </c>
       <c t="s" r="F2">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="G2">
         <v>0</v>
@@ -1121,7 +1388,7 @@
         <v>8</v>
       </c>
       <c t="s" r="N2">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="O2">
         <v>12</v>
@@ -1132,7 +1399,7 @@
         <v>2</v>
       </c>
       <c t="s" r="B3">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="C3">
         <v>22</v>
@@ -1144,7 +1411,7 @@
         <v>1</v>
       </c>
       <c t="s" r="F3">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="G3">
         <v>6</v>
@@ -1156,10 +1423,48 @@
         <v>3</v>
       </c>
       <c t="s" r="N3">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="O3">
         <v>14</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c t="s" r="B4">
+        <v>42</v>
+      </c>
+      <c r="C4">
+        <v>29</v>
+      </c>
+      <c r="D4">
+        <v>28</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c t="s" r="F4">
+        <v>47</v>
+      </c>
+      <c r="G4">
+        <v>5</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="J4">
+        <v>21</v>
+      </c>
+      <c r="K4">
+        <v>1</v>
+      </c>
+      <c t="s" r="N4">
+        <v>48</v>
+      </c>
+      <c r="O4">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -1225,7 +1530,7 @@
         <v>1</v>
       </c>
       <c t="s" r="B2">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="C2">
         <v>9</v>
@@ -1237,7 +1542,7 @@
         <v>2</v>
       </c>
       <c t="s" r="F2">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="G2">
         <v>5</v>
@@ -1261,7 +1566,7 @@
         <v>0</v>
       </c>
       <c t="s" r="N2">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="O2">
         <v>7</v>
@@ -1272,7 +1577,7 @@
         <v>2</v>
       </c>
       <c t="s" r="B3">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="C3">
         <v>8</v>
@@ -1284,7 +1589,7 @@
         <v>1</v>
       </c>
       <c t="s" r="F3">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="G3">
         <v>1</v>
@@ -1308,9 +1613,56 @@
         <v>7</v>
       </c>
       <c t="s" r="N3">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="O3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c t="s" r="B4">
+        <v>49</v>
+      </c>
+      <c r="C4">
+        <v>8</v>
+      </c>
+      <c r="D4">
+        <v>7</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c t="s" r="F4">
+        <v>54</v>
+      </c>
+      <c r="G4">
+        <v>6</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c t="s" r="N4">
+        <v>55</v>
+      </c>
+      <c r="O4">
         <v>10</v>
       </c>
     </row>

</xml_diff>